<commit_message>
Many improvements and new functionality:  - Implemented button editor  - Added OSC support  - Added key rgb backlight control  - Added key names to the OLED  - Implemented USB configuration messages  - Fixed json profile saving  - Added autosaving  - Fixed bindings and event driven stuff  - Added OnExit handler  - Added automatic USB disconnection detection  - Improved performance of the Arduino code  - Improved graphics on the OLED  - Refactoring
</commit_message>
<xml_diff>
--- a/KeyLayout.xlsx
+++ b/KeyLayout.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{99FE00DB-FB11-41E8-AEFE-3E4711D99650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D70EC401-0F77-4FE3-8CF8-840A1307D55C}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D70EC401-0F77-4FE3-8CF8-840A1307D55C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
   <dimension ref="B1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>